<commit_message>
added Japanese translation of tool summary
added Japanese translation of tool summary
</commit_message>
<xml_diff>
--- a/subgroups/sbom-sg/outcomes/SBOM/SBOMTools/LearnSBOM/LearnSBOMList.xlsx
+++ b/subgroups/sbom-sg/outcomes/SBOM/SBOMTools/LearnSBOM/LearnSBOMList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sonyjpn-my.sharepoint.com/personal/hiroyuki_fukuchi_sony_com/Documents/ドキュメント/OpenChain/SBOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="604" documentId="8_{0F481742-EC34-4620-BA6D-267154DAC474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FE4140E-01C9-4E7F-B619-BFCA77B30865}"/>
+  <xr:revisionPtr revIDLastSave="609" documentId="8_{0F481742-EC34-4620-BA6D-267154DAC474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9479E97-C23A-470B-9ABE-3B3E8793D418}"/>
   <bookViews>
-    <workbookView xWindow="504" yWindow="960" windowWidth="20772" windowHeight="10152" activeTab="3" xr2:uid="{627C03B7-2A37-4A7C-9FB2-07470DF8D28A}"/>
+    <workbookView xWindow="1464" yWindow="1464" windowWidth="20772" windowHeight="10152" activeTab="3" xr2:uid="{627C03B7-2A37-4A7C-9FB2-07470DF8D28A}"/>
   </bookViews>
   <sheets>
     <sheet name="SBOM_Utility_Tools" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="518">
   <si>
     <t>https://www.youtube.com/@LearnSBOM/playlistsその他は以下です。</t>
   </si>
@@ -8089,12 +8089,431 @@
     </r>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>概要</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>Sonatype Nancyは、Go環境向けのセキュリティスキャナです。このビデオでは、SonatypeのOSSインデックス脆弱性データベースを使用して脆弱な依存関係を検索する依存関係スキャナーツールについて説明します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>概要
+Jakeは、マニフェストファイルを介してCycloneDX SBOMを生成し、Sonatypeデータベースでセキュリティスキャンを実行するPythonパッケージです。このビデオでは、生成機能とスキャン機能の使用方法について説明します。
+⚠️編集9/26/2022 ⚠️ JakeはSonatypeの 「コントリビューション」 ですが、Sonatypeではサポートされていません。詳細情報:https://github.com/sonatype-nexus-com ...</t>
+    </r>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+Retire.jsはJSプロジェクト用のオープンソースのセキュリティツールで、Webブラウザー拡張機能としてインストールできます。このデモでは、ブラウザー拡張機能とリアルタイム脆弱性分析Webサイトのいくつかの機能について説明します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+Pip-Auditは、脆弱なパッケージをスキャンするPythonプロジェクトスキャナーです。このビデオでは、さまざまなpythonプロジェクトと環境をスキャンする方法について説明します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+ShiftLeft Scanはオープンソースセキュリティツールであり、ローカルプロジェクトの脆弱性をスキャンするためにコンテナー内で実行されるDockerイメージです。これらのスキャンは、結果のエグゼクティブサマリーと、脆弱なコンポーネントハッシュやシークレットの監査結果を含むその他の情報を生成します。このビデオでは、ツールの操作方法といくつかの機能の使用方法について説明します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t xml:space="preserve">概要
+OSS Review Toolkit (ORT) は、プロジェクトディレクトリをスキャンしてさまざまな形式の一連のセキュリティレポートを生成できるオールインワンCLIプロジェクトユーティリティツールです。このビデオでは、Dockerといくつかのコマンドを使用してORTをビルドする方法を示します。 </t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+Coinbase Salusは、さまざまなプロジェクトに脆弱性や不適切なコーディングがないかをスキャンするセキュリティスキャンツールだ。このビデオでは、2つの異なるプロジェクトでツールを使用し、結果を分析するデモを行います。また、セキュリティニーズに合わせてSalus用のカスタム構成ファイルを作成する方法についても説明します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+オープンソース脆弱性検出器は、プロジェクトのロックファイルを使用して脆弱性スキャンを実行するバイナリです。このビデオでは、バイナリを使用して一連のプロジェクトをスキャンする方法について説明します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+TernはLinux上のDockerイメージ用のSBOMジェネレータです。Ternはさまざまなシェルスクリプトを使用して、Dockerコンテナの構築に使用されるさまざまなレイヤを解析し、各レイヤの依存関係に関する非常に詳細なレポートを作成します。また、このツールはSPDXやCycloneDX SBOMを含む一連のSBOMを作成することもできる。さらに、TernにはDocker-Lock機能があり、Dockerfileを他のロックファイルと同様に実行時により正確なバージョンに変換する。このビデオでは、Ternを最大限に活用する方法を説明します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+OchronaCLIは、Pythonプロジェクトをスキャンして脆弱なパッケージを検出する脆弱性スキャナーです。このツールには、CycloneDX SBOMを生成する機能など、環境のニーズに最適な機能が多数用意されています。このビデオでは、OchronaCLIを使用してPythonコードの脆弱性をスキャンする方法について説明します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+Grypeは、プロジェクトとSBOMをスキャンして安全であることを確認するバイナリツールです。Grypeには、大規模で適切に管理されたデータベースがあり、最適に機能するようにGrypeを設定するための一連のカスタマイズ可能なオプションがあります。このビデオでは、Grypeの基本とプロジェクトでの使用方法について説明します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>説明
+AuditJSは、ノードプロジェクトの脆弱性スキャナーを簡単に使用できるCLIツールです。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>Kicsは、さまざまなインフラストラクチャと互換性のある脆弱性、コンプライアンス、およびインフラストラクチャの構成ミスをスキャンするツールです。Kicsは、Azure、AWS、Bitbucketなど、多くのプラグインでCI/CDをサポートしている。このビデオでは、インストールと脆弱性スキャンの機能に焦点を当て、Kicsのクエリの作成方法とKicsのユースケースについて説明します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t xml:space="preserve">このビデオでは、Cloud Native Computing Foundationによって開発されたツールであるCosignについて詳しく説明します。Cosignは、サプライチェーンの透明性を高め、組織がソフトウェアイメージの認証と整合性を検証できるようにするイメージ署名を可能にします。ソフトウェア部品表 (SBOMS) は、イメージの共同署名と統合することもでき、トレーサビリティによってリスク管理を向上させることができます。 </t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>説明
+包括的で汎用性の高いセキュリティスキャナであるTrivyのデモをご覧ください。Trivyは、セキュリティの問題を探すスキャナーと、それらの問題を見つけることができるターゲットを持っています。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+CDX-BOM-Repoは、CycloneDX SBOM用にカスタマイズ可能なSBOMリポジトリを作成するDockerコンテナです。このビデオでは、コンテナを設定する方法と、Repoにアクセス/管理する方法について説明します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+Markdown SBOM Tool (mdbom) は、CycloneDX SBOMを取得してmarkdownファイルに変換するPythonパッケージです。このビデオでは、既定で提供されている.mdテンプレートを使用してSBOMを変換し、結果を表示する方法について説明します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+SPDX Javaは、SPDX SBOMを処理するために使用されるバイナリ・ツールです。このツールは、SPDX SBOMの生成、変換、比較、検証および表示を行うことができます。このビデオでは、これらのすべての機能をデモンストレーションし、結果を説明します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+CycloneDX Web Appは、ローカルまたはCycloneDX GitHubページを通じて実行されるWebアプリケーションで、GUIを通じて基本的なSBOMツールを簡単に使用できます。このビデオでは、Webサイトへのアクセス方法といくつかの機能について説明します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+CycloneDX CLIは、CycloneDX SBOMの生成、変換、および解析を行う、複数のオペレーティング・システムで使用可能なバイナリ・ツールです。このビデオでは、SBOMで基本的な関数を使用する方法を示し、結果について詳しく説明します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+CycloneDX Core for Javaは、カスタムSBOMファイルの作成と解析を可能にするMavenプラグインです。このビデオでは、このライブラリの基本を説明するために、2つのJavaプログラムについて説明します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+CycloneDX for NPM GitHub Actionは、CycloneDX for NPMを使用するGitHub Actionです。このビデオでは、このツールをGitHubワークフローに組み込む方法を示します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+Open Source Vulnerability Databaseは公開されているオープンソースのデータベースで、さまざまなエコシステムから3万以上の脆弱性が保存されています。このビデオでは、データベース自体とOSV APIの使用方法について説明します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+SCANOSS Audit Workbenchは、プロジェクトの内容を視覚的に表示するGUIツールです。このビデオでは、レポートを生成して分析する方法について説明します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">概要
+SPDXオンラインツールは、ツールをダウンロードまたは設定することなく、SPDX SBOMを簡単に操作できるWebサイトです。
+❗更新❗
+SPDXオンラインツールには、録画時にはなかった 「NTIA適合性チェッカー」 機能が追加されました。この機能は、SPDX SBOMを取得し、NTIAの 「SBOMの最小要素」 要件を満たしているかどうかをチェックします。
+🎯ソースコード:https://github.com/spdx/ntia-conforma ...
+🎯"SBOMの最小要素":https://www.ntia.doc.gov/files/ntia/p ...
+</t>
+    </r>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>説明
+dtrack-auditは、Dependency Track APIと連携してDependency Trackプロジェクトを設定および管理するGoツールです。使用する環境変数が多数あり、CI/CDパイプラインでの作業に最適です。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>説明
+CycloneDX Pythonライブラリは、Pythonで独自のカスタムSBOMツールを構築する優れた方法です。以前取り上げた既存のOSSツールの多くは、これらのライブラリを利用しています。このデモでは、CycloneDX Pythonライブラリの使用方法のほんの一部を示します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>SBOMToolsは、SBOMからコンポーネントのリスト、検索、追加、削除を実行できる4-in-1 SBOMユーティリティです。SBOMToolsはCycloneDXとSPDXの両方のJSON形式で動作します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>SBOM品質スコアは、SBOMの品質を評価するためのコマンドラインツールです。SBOMqsは、SBOMの消費性を評価します。スコアが高いほど、SBOMの消耗性が高くなります。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>Hopprは、ソフトウェア部品表 (SBOM) およびセキュアソフトウェアサプライチェーン (S3C) ユーティリティキットです。シンプルなプラグインアーキテクチャで構築されたHopprは、デジタル資産を収集、処理、バンドルして、ある本番環境から別の本番環境への転送を合理化できます。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>SBOM2DOCを使用すると、さまざまなSBOM形式から専門的で読みやすいドキュメントを生成できます。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>このビデオでは、ソフトウェアのセキュリティと信頼性を評価するためのツールであるeBayのSBOMスコアカードを詳しく見ていきます。その評価基準を探求し、情報に基づいた意思決定に活用する方法を発見し、サプライチェーンのセキュリティを強化する上での重要な役割を理解するために、私たちに参加してください。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>説明
+このデモでは、SPDXおよびCycloneDX形式のディレクトリからSBOMを生成するために設計されたオープンソースツールであるSBOM4Filesについて説明します。このツールは、ディレクトリ内のファイルを識別し、ライセンスおよび著作権情報のリストをコンパイルします。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>説明
+このビデオでは、包括的なチェックを通じてSBOMコンテンツの品質をレポートするコマンドラインインターフェイスであるSBOM監査ツールについて説明します。このツールは、タグ値、JSON、YAML形式のSPDX SBOMと、JSON形式のCycloneDX SBOMをサポートしています。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>説明
+SCANOSS API/Engineと対話するための簡単に使用可能なモジュールを提供するツールであるSCANOSS JSのデモに参加してください。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CycloneDX for Webpackは、JavaScript、Angular、React Webpackバンドル用のCycloneDX SBOMをすばやく生成できるWebpackプラグインです。 </t>
+  </si>
+  <si>
+    <t>ScanCodeツールキットは、ライセンス、著作権、パッケージマニフェスト、直接の依存関係などを検出します。主に、ライセンスの検出に使用されます。結果は、JSON、HTML、CSV、SPDX、またはJinjaテンプレートを使用したカスタム形式で保存できます。Scancodeツールキットは、Eclipse FoundationやOSS Review Toolkitなど、多くのグループやプロジェクトで使用されています。</t>
+  </si>
+  <si>
+    <t>CycloneDX Mavenは、Mavenを使用するJavaプロジェクト用のプラグインです。このビデオでは、コマンドプロンプトからいくつかのコマンドを使用して、このツールでSBOMを生成する方法を説明します。さらに、CycloneDX SBOMの構成要素についても説明します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+CycloneDX-Conanは、Conanを使用してCおよびC++プロジェクト用のCycloneDX SBOMを生成するPythonパッケージです。このビデオでは、ツールの使用方法と、ツールの使用中に発生するいくつかの問題の解決方法を示します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t xml:space="preserve">概要
+cdxgenはCycloneDX SBOMの生成に使用できるインストール可能なパッケージです。このツールはCLIを使用し、非常に簡単に使用できます。このビデオでは、いくつかのコマンドだけでSBOMを生成する方法について簡単に説明します。
+</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+CycloneDX for Pythonは、Pythonプロジェクト用のCycloneDX SBOMを生成するPythonパッケージです。開発環境に合わせて、さまざまな場所から実行できます。このビデオでは、CycloneDX for Pythonを使用してSBOMを生成する方法について説明します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+SPDX SBOM Generatorは、CLIを使用してSPDXおよびJSON形式のSPDX SBOMを生成するバイナリ(Mac、Linux、Windowsで利用可能)です。このビデオでは、ツールの基本的な使用方法を示し、SPDXの結果を分析します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+CycloneDXはのSBOMジェネレータです。NETプロジェクトを使用します。slnファイルをスキャンすることも、.csprojファイルを再帰的にスキャンすることもできます。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+CycloneDX for NPMは、ノードのSBOMジェネレータです。JSプロジェクト。NPMからインストールして使用できます。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+Microsoft Salusは、の実行可能なSBOM生成および検証ツールです。NETプロジェクトに対応しており、Windows、Linux、MacOSで利用できる。このツールは、指定されたディレクトリ内の.csprojファイルをスキャンし、SPDX形式のSBOMを生成します。このビデオでは、コマンドを正しく設定し、結果を分析する方法について説明します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t xml:space="preserve">概要
+これは、Dockerイメージ用のコマンドラインSBOMジェネレータです。 </t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+CycloneDX PHP Composer Pluginは、Composer依存関係マネージャを使用してSBOMを作成するPHPプロジェクト用です。このビデオでは、composerを使用してツールをインストールし、composerのロックファイルを使用してSBOMを生成する方法を説明します。おまけとして、このツールを使用するGitHubアクションの使用方法も説明します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+Syftは、DockerイメージとプロジェクトからSyft、SPDX、CycloneDX SBOMを生成するバイナリツールです。このツールは幅広い言語をサポートしており、作業環境に非常に柔軟に対応できます。このビデオでは、Syftを使用して独自のプロジェクトのSBOMを作成する方法について説明します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+JBOMは、静的および実行時バイナリからCycloneDX SBOMを生成できるjar実行可能ファイルです。このツールはソースコードへのアクセスを必要としないため、サードパーティ製またはクローズドソースのソフトウェアを使用する開発パイプラインを保護する際に貴重なリソースとなります。このビデオでは、JBOMを使用してこれらのSBOMを生成する方法について説明します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+apt2sbomは、インストールされたaptパッケージからSPDXおよびCycloneDX SBOMを生成するために使用できる単純なpythonパッケージです。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+SyftとGrypeには、ワークフローを改善するGitHub Actionsもある。これらは簡単に実装でき、ワークフローの自律性を維持するのに役立ちます。このビデオでは、各アクションの使用方法と、各ツールを最大限に活用するための最適な組み合わせについて詳しく説明します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>説明
+SPDX Maven PluginはMavenプロジェクト用のプラグインです。このプラグインには、Maven構築プロセスの一部として詳細なSPDX SBOMを作成するための多数の構成オプションがあります。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>説明
+WpBomは、WordPressサーバーにインストールされているすべてのプラグインとテーマを含むSBOMを自動的に生成するWordPressプラグインです。これらのSBOMは、プラグインまたはテーマが削除されるたびに、Dependency Trackサーバーにシームレスにアップロードできます。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>説明
+⚠️注⚠️このツールは古いCyclondeDXスキーマを使用しており、そのまま実行するといくつかの問題がありますが、修正を行っています。
+CDX Bower BOMは、Bowerを使用するJavascriptプロジェクト用のCycloneDX SBOMを生成するCLIツールです。CLIツールは、SBOMをマージするという追加機能を備えており、すばやく簡単に使用できます。 
+インストール
+Node.js v 8.0.0+(ダウンロード|Node.js)
+Bower (npm install-g bower)
+cdx-bower-bom (npm install-g cdx-bower-bom)
+バグ修正
+cdx-bower-bomグローバルインストール場所 (%appdata%/npm/node_modules/cdx-bower-bom/bin/cdx-bower-bom)</t>
+    </r>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>説明
+CycloneDx Gradle Pluginは、Gradle/Kotlinプロジェクト用のシンプルなプラグインです。このツールを使用して、CycloneDX SBOMをJSON形式とXML形式の両方で生成できます。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+SCANOSS Python Toolは、コマンドライン、パッケージ、またはDocker経由で使用できるPythonパッケージです。SCANOSS SCA APIを使用してWebをスクレイピングし、CycloneDXやSPDX-Liteなどの多数のSBOMを構築します。さらに、フィンガープリントアルゴリズムを使用して、ソースコードに一意のデジタルフィンガープリントを作成します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>CycloneDX for Rust Cargoは、Rust CargoプロジェクトのSBOMを生成するコマンドラインツールです。これはCargoプラグインで、cargo.tomlファイルを使用してSBOMを生成します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>CycloneDX-GoModは、コマンドラインツールとして使用できるSBOMジェネレーターであり、GitHub Action、GoReleaser、Docker、およびライブラリの実装を通じて使用することもできます。スキャンしようとしているプロジェクトに応じて、アプリケーション、モジュール、バイナリの3つのサブコマンドがあります。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>OpenRewriteは、大規模なソースコードリファクタリングエコシステムで最もよく知られていますが、このツールを使用してSBOMを生成することもできます。
+角かっこXSS攻撃を防ぐためにyoutubeの説明に入れることはできません。だから、この動画で使われているコードを挿入することはできません。代わりに、コードはOpenrewriteのドキュメントにあります (以下の参考文献にあります) 。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>ビルド情報goは、Go、Maven、Gradle、NPM、NuGet、dotnet、yarn、pip、pipenv、および詩プロジェクトのSBOMやその他のビルド情報を生成するgoで記述されたジェネレーターです。また、goプロジェクト内からビルド情報を生成できるgoのAPIエンドポイントも備えています。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>CycloneDX Ruby Gemは、Gemfile.lockをスキャンし、CycloneDX v1.1 XML SBOMを生成するRubyプロジェクト用のSBOMジェネレータです。このツールは2年以上更新されていないため、代わりにCDXGenを使用することをお勧めします。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>Lib4SBOMは、ソフトウェア部品表 (SBOM) を解析および生成するPythonライブラリです。SPDXおよびCycloneDXフォーマットをサポートしています。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CycloneDX-goはGoプロジェクト用の非常にシンプルなSBOMジェネレータです;CycloneDxバージョン1.1のみが生成されます。Goバージョン1.11以降が必要で、Go.modフォルダがあるプロジェクトでのみ動作します。 </t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>Gobomは、Go、NPM、Cocoapods、Gradleプロジェクト用のコマンドラインSBOMジェネレータです。依存関係追跡プラグインとしても使用でき、gobomが現在のニーズに合わない場合は、カスタムジェネレーターを追加できます。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>コヴェナントは、コマンドラインインターフェイスでソースコードアーティファクトを使用するSBOM生成ツールです。CycloneDX形式とSPDX形式の両方のSBOMファイルを生成できます。コヴェナントは、SBOMファイルのHTMLレポートを作成したり、SBOMファイルのコンプライアンスチェックを実行したりすることもできます。
+NOTE:規約では、可能な限り正確な分析を行うために、すべてのプロジェクトが構築され、すべての依存関係が復元されている必要があります。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>koはGoアプリケーション用のシンプルで高速なコンテナイメージビルダーです。イメージを構築するためにdockerを必要とせず、Kubernetesアプリケーションのための強力なツールです。 
+これは、OSベースイメージに多くの依存関係がない単一のGoアプリケーションを含むイメージに最も便利です。
+KoはデフォルトでSPDX SBOMを生成し、CycloneDX SBOMを作成することもできます。CosignはSBOMをレジストリからプルするために使用されます。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>CycloneDX CocoapodsはCycloneDX v1.4用のCocoapods SBOMジェネレータです。SBOMはXML形式でのみ生成され、生成にはPodfileが必要です。また、完全に正確なSBOMを生成するには手動入力が必要で、CI/CD統合はありません。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>説明
+このデモでは、Pythonプロジェクトのソフトウェア部品表を生成するために設計されたオープンソースツールであるSBOM4Pythonについて説明します。SPDXおよびCycloneDXフォーマットをサポートしているため、このツールを使用して結果を分析する方法を説明します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>説明
+Elang/ElixirプロジェクトのSBOMSを生成するツールであるCycloneDX for Erlang/Elixir (Rebar3) のデモに参加しましょう。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t xml:space="preserve">説明
+このビデオでは、SBOM4Rustのデモを行います。Pythonを使用して、Rustアプリケーション用のSBOMをSPDXおよびCycloneDXフォーマットで生成するツール。 </t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>説明
+このデモでは、インストールされたアプリケーションまたは完全なシステムインストールのSBOM (Software Bill of Materials) をSPDXやCycloneDXなどのさまざまな形式で生成するツールである、Distro2SBOMについて説明します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>説明
+今日は、SBT (Scala) プロジェクトのCycloneDX SBOMを作成するプラグインであるSBT-BOMのデモを行います。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>説明
+今日は、デモと概念実証を目的として、SPDX、CycloneDX、SWID形式のSBOMを生成するツールであるSwiftBOMをレビューします。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>説明
+GH (GitHub) SBOMのデモに参加してください;依存関係グラフの情報を使用してGitHubリポジトリのJSON SBOM (SPDXまたはCycloneDX形式) を出力するgh CLI拡張機能です。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+SPDXCycloneは、CycloneDX形式のSBOMをSPDX SBOMに変換して戻すCLIを介した.jar実行可能ファイルです。このビデオでは、ファイルを変換するプロセスの使用方法を示し、CycloneDXがSPDXにどのようにマッピングされるかを説明します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>概要
+SPDX Pythonは、SPDX形式のファイルを解析および変換するために使用されるPythonパッケージです。このビデオでは、生成と解析の例をいくつか示します。</t>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>概要
+SPDXオンラインツールは、ツールをダウンロードまたは設定することなく、SPDX SBOMを簡単に操作できるWebサイトです。
+❗更新❗
+SPDXオンラインツールには、録画時にはなかった 「NTIA適合性チェッカー」 機能が追加されました。この機能は、SPDX SBOMを取得し、NTIAの 「SBOMの最小要素」 要件を満たしているかどうかをチェックします。
+🎯ソースコード:https://github.com/spdx/ntia-conforma ...
+🎯"SBOMの最小要素":https://www.ntia.doc.gov/files/ntia/p ...</t>
+    </r>
+    <phoneticPr fontId="10"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8160,6 +8579,18 @@
       <color theme="1"/>
       <name val="Segoe UI Emoji"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="3">
@@ -8267,7 +8698,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -8318,6 +8749,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -17278,10 +17718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54119C77-527F-4903-B6A0-019866776B69}">
-  <dimension ref="A3:G27"/>
+  <dimension ref="A3:H27"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -17290,18 +17730,19 @@
     <col min="2" max="2" width="19.5" style="3" customWidth="1"/>
     <col min="3" max="3" width="15" style="3" customWidth="1"/>
     <col min="4" max="4" width="31.796875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="39.296875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="34.59765625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="42.19921875" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="8.796875" style="3"/>
+    <col min="5" max="5" width="39.296875" style="17" customWidth="1"/>
+    <col min="6" max="6" width="39.296875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="34.59765625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="42.19921875" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="8.796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D3" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>171</v>
       </c>
@@ -17314,17 +17755,20 @@
       <c r="D5" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="18" t="s">
+        <v>440</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="210" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" ht="210" x14ac:dyDescent="0.45">
       <c r="A6" s="11" t="s">
         <v>55</v>
       </c>
@@ -17337,17 +17781,20 @@
       <c r="D6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="19" t="s">
+        <v>456</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="135" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" ht="135" x14ac:dyDescent="0.45">
       <c r="A7" s="12"/>
       <c r="B7" s="9" t="s">
         <v>106</v>
@@ -17358,17 +17805,20 @@
       <c r="D7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="19" t="s">
+        <v>457</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="150" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" ht="150" x14ac:dyDescent="0.45">
       <c r="A8" s="12"/>
       <c r="B8" s="9" t="s">
         <v>107</v>
@@ -17379,17 +17829,20 @@
       <c r="D8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="19" t="s">
+        <v>458</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="135" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" ht="135" x14ac:dyDescent="0.45">
       <c r="A9" s="12"/>
       <c r="B9" s="9" t="s">
         <v>108</v>
@@ -17400,17 +17853,20 @@
       <c r="D9" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="19" t="s">
+        <v>459</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="150" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" ht="150" x14ac:dyDescent="0.45">
       <c r="A10" s="12"/>
       <c r="B10" s="9" t="s">
         <v>109</v>
@@ -17421,17 +17877,20 @@
       <c r="D10" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="19" t="s">
+        <v>460</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="105" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" ht="105" x14ac:dyDescent="0.45">
       <c r="A11" s="12"/>
       <c r="B11" s="9" t="s">
         <v>110</v>
@@ -17442,17 +17901,20 @@
       <c r="D11" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="19" t="s">
+        <v>461</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="150" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" ht="150" x14ac:dyDescent="0.45">
       <c r="A12" s="12"/>
       <c r="B12" s="9" t="s">
         <v>111</v>
@@ -17463,17 +17925,20 @@
       <c r="D12" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="19" t="s">
+        <v>462</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="H12" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="195" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" ht="195" x14ac:dyDescent="0.45">
       <c r="A13" s="12"/>
       <c r="B13" s="9" t="s">
         <v>112</v>
@@ -17484,17 +17949,20 @@
       <c r="D13" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="19" t="s">
+        <v>463</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="G13" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="165" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" ht="165" x14ac:dyDescent="0.45">
       <c r="A14" s="12"/>
       <c r="B14" s="9" t="s">
         <v>113</v>
@@ -17505,17 +17973,20 @@
       <c r="D14" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="19" t="s">
+        <v>464</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="183.6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" ht="255" x14ac:dyDescent="0.45">
       <c r="A15" s="12"/>
       <c r="B15" s="9" t="s">
         <v>114</v>
@@ -17526,17 +17997,20 @@
       <c r="D15" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="19" t="s">
+        <v>465</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="G15" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="H15" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="210" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" ht="210" x14ac:dyDescent="0.45">
       <c r="A16" s="12"/>
       <c r="B16" s="9" t="s">
         <v>115</v>
@@ -17547,17 +18021,20 @@
       <c r="D16" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="19" t="s">
+        <v>466</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="H16" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="150" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" ht="150" x14ac:dyDescent="0.45">
       <c r="A17" s="12"/>
       <c r="B17" s="9" t="s">
         <v>116</v>
@@ -17568,17 +18045,20 @@
       <c r="D17" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="19" t="s">
+        <v>467</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="G17" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="H17" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="135" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" ht="135" x14ac:dyDescent="0.45">
       <c r="A18" s="12"/>
       <c r="B18" s="9" t="s">
         <v>117</v>
@@ -17589,17 +18069,20 @@
       <c r="D18" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="19" t="s">
+        <v>468</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="G18" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="H18" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="195" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" ht="195" x14ac:dyDescent="0.45">
       <c r="A19" s="12"/>
       <c r="B19" s="9" t="s">
         <v>137</v>
@@ -17610,17 +18093,20 @@
       <c r="D19" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="19" t="s">
+        <v>469</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="G19" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="H19" s="4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="120" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" ht="120" x14ac:dyDescent="0.45">
       <c r="A20" s="12"/>
       <c r="B20" s="9" t="s">
         <v>118</v>
@@ -17631,17 +18117,20 @@
       <c r="D20" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="19" t="s">
+        <v>470</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="G20" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="H20" s="4" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="120" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" ht="120" x14ac:dyDescent="0.45">
       <c r="A21" s="12"/>
       <c r="B21" s="9" t="s">
         <v>119</v>
@@ -17652,17 +18141,20 @@
       <c r="D21" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="19" t="s">
+        <v>454</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="G21" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="H21" s="4" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="105" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" ht="105" x14ac:dyDescent="0.45">
       <c r="A22" s="12"/>
       <c r="B22" s="9" t="s">
         <v>120</v>
@@ -17673,17 +18165,20 @@
       <c r="D22" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="19" t="s">
+        <v>471</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="G22" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="H22" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="150" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" ht="150" x14ac:dyDescent="0.45">
       <c r="A23" s="12"/>
       <c r="B23" s="9" t="s">
         <v>121</v>
@@ -17694,17 +18189,20 @@
       <c r="D23" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="19" t="s">
+        <v>472</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="G23" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="H23" s="4" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="120" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" ht="120" x14ac:dyDescent="0.45">
       <c r="A24" s="12"/>
       <c r="B24" s="9" t="s">
         <v>122</v>
@@ -17715,17 +18213,20 @@
       <c r="D24" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="19" t="s">
+        <v>473</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="G24" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="H24" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="225" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" ht="225" x14ac:dyDescent="0.45">
       <c r="A25" s="12"/>
       <c r="B25" s="9" t="s">
         <v>123</v>
@@ -17736,17 +18237,20 @@
       <c r="D25" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="19" t="s">
+        <v>474</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="G25" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="H25" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="120" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" ht="120" x14ac:dyDescent="0.45">
       <c r="A26" s="13"/>
       <c r="B26" s="9" t="s">
         <v>124</v>
@@ -17757,17 +18261,20 @@
       <c r="D26" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="19" t="s">
+        <v>475</v>
+      </c>
+      <c r="F26" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="G26" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="H26" s="4" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" s="14"/>
       <c r="D27" s="7"/>
     </row>
@@ -17805,10 +18312,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89B6520E-B16E-496E-94D2-3598A03EA2EA}">
-  <dimension ref="A3:G50"/>
+  <dimension ref="A3:H50"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -17816,18 +18323,19 @@
     <col min="1" max="1" width="14" style="3" customWidth="1"/>
     <col min="2" max="3" width="19.5" style="3" customWidth="1"/>
     <col min="4" max="4" width="31.796875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="41.09765625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="34.59765625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="42.19921875" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="8.796875" style="3"/>
+    <col min="5" max="5" width="41.09765625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="41.09765625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="34.59765625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="42.19921875" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="8.796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D3" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>171</v>
       </c>
@@ -17840,17 +18348,20 @@
       <c r="D5" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="18" t="s">
+        <v>440</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="105" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" ht="105" x14ac:dyDescent="0.45">
       <c r="A6" s="11" t="s">
         <v>212</v>
       </c>
@@ -17863,17 +18374,20 @@
       <c r="D6" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="19" t="s">
+        <v>478</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="135" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" ht="150" x14ac:dyDescent="0.45">
       <c r="A7" s="12"/>
       <c r="B7" s="4" t="s">
         <v>217</v>
@@ -17884,17 +18398,20 @@
       <c r="D7" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="19" t="s">
+        <v>442</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="135" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" ht="135" x14ac:dyDescent="0.45">
       <c r="A8" s="12"/>
       <c r="B8" s="4" t="s">
         <v>221</v>
@@ -17905,17 +18422,20 @@
       <c r="D8" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="19" t="s">
+        <v>479</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="150" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" ht="150" x14ac:dyDescent="0.45">
       <c r="A9" s="12"/>
       <c r="B9" s="4" t="s">
         <v>109</v>
@@ -17926,17 +18446,20 @@
       <c r="D9" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="19" t="s">
+        <v>460</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="105" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" ht="105" x14ac:dyDescent="0.45">
       <c r="A10" s="12"/>
       <c r="B10" s="4" t="s">
         <v>228</v>
@@ -17947,17 +18470,20 @@
       <c r="D10" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="19" t="s">
+        <v>480</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="135" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" ht="135" x14ac:dyDescent="0.45">
       <c r="A11" s="12"/>
       <c r="B11" s="4" t="s">
         <v>229</v>
@@ -17968,17 +18494,20 @@
       <c r="D11" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="19" t="s">
+        <v>481</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="120" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" ht="120" x14ac:dyDescent="0.45">
       <c r="A12" s="12"/>
       <c r="B12" s="4" t="s">
         <v>233</v>
@@ -17989,17 +18518,20 @@
       <c r="D12" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="19" t="s">
+        <v>482</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="H12" s="4" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="165" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" ht="165" x14ac:dyDescent="0.45">
       <c r="A13" s="12"/>
       <c r="B13" s="4" t="s">
         <v>238</v>
@@ -18010,17 +18542,20 @@
       <c r="D13" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="19" t="s">
+        <v>446</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="G13" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="120" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" ht="120" x14ac:dyDescent="0.45">
       <c r="A14" s="12"/>
       <c r="B14" s="4" t="s">
         <v>241</v>
@@ -18031,17 +18566,20 @@
       <c r="D14" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="19" t="s">
+        <v>483</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="120" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" ht="120" x14ac:dyDescent="0.45">
       <c r="A15" s="12"/>
       <c r="B15" s="4" t="s">
         <v>244</v>
@@ -18052,17 +18590,20 @@
       <c r="D15" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="19" t="s">
+        <v>484</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="G15" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="H15" s="4" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="135" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" ht="135" x14ac:dyDescent="0.45">
       <c r="A16" s="12"/>
       <c r="B16" s="4" t="s">
         <v>248</v>
@@ -18073,17 +18614,20 @@
       <c r="D16" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="19" t="s">
+        <v>485</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="H16" s="4" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="165" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" ht="165" x14ac:dyDescent="0.45">
       <c r="A17" s="12"/>
       <c r="B17" s="4" t="s">
         <v>252</v>
@@ -18094,17 +18638,20 @@
       <c r="D17" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="19" t="s">
+        <v>486</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="G17" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="H17" s="4" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="255" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" ht="255" x14ac:dyDescent="0.45">
       <c r="A18" s="12"/>
       <c r="B18" s="4" t="s">
         <v>256</v>
@@ -18115,17 +18662,20 @@
       <c r="D18" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="19" t="s">
+        <v>487</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="G18" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="H18" s="4" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="210" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" ht="210" x14ac:dyDescent="0.45">
       <c r="A19" s="12"/>
       <c r="B19" s="4" t="s">
         <v>260</v>
@@ -18136,17 +18686,20 @@
       <c r="D19" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="19" t="s">
+        <v>488</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="G19" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="H19" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="255" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" ht="255" x14ac:dyDescent="0.45">
       <c r="A20" s="12"/>
       <c r="B20" s="4" t="s">
         <v>262</v>
@@ -18157,17 +18710,20 @@
       <c r="D20" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="G20" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="H20" s="4" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="165" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" ht="165" x14ac:dyDescent="0.45">
       <c r="A21" s="12"/>
       <c r="B21" s="4" t="s">
         <v>266</v>
@@ -18178,17 +18734,20 @@
       <c r="D21" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="19" t="s">
+        <v>489</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="G21" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="H21" s="4" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="150" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" ht="150" x14ac:dyDescent="0.45">
       <c r="A22" s="12"/>
       <c r="B22" s="4" t="s">
         <v>267</v>
@@ -18199,17 +18758,20 @@
       <c r="D22" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="19" t="s">
+        <v>490</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="G22" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="H22" s="4" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="360" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" ht="360" x14ac:dyDescent="0.45">
       <c r="A23" s="12"/>
       <c r="B23" s="4" t="s">
         <v>275</v>
@@ -18220,17 +18782,20 @@
       <c r="D23" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="19" t="s">
+        <v>491</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="G23" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="H23" s="4" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="120" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" ht="120" x14ac:dyDescent="0.45">
       <c r="A24" s="12"/>
       <c r="B24" s="4" t="s">
         <v>277</v>
@@ -18241,17 +18806,20 @@
       <c r="D24" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="19" t="s">
+        <v>492</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="G24" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="H24" s="4" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="180" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" ht="180" x14ac:dyDescent="0.45">
       <c r="A25" s="12"/>
       <c r="B25" s="4" t="s">
         <v>282</v>
@@ -18262,17 +18830,20 @@
       <c r="D25" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="19" t="s">
+        <v>493</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="G25" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="H25" s="4" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="252.6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" ht="285" x14ac:dyDescent="0.45">
       <c r="A26" s="12"/>
       <c r="B26" s="4" t="s">
         <v>286</v>
@@ -18283,17 +18854,20 @@
       <c r="D26" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="19" t="s">
+        <v>494</v>
+      </c>
+      <c r="F26" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="G26" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="H26" s="4" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="120" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" ht="120" x14ac:dyDescent="0.45">
       <c r="A27" s="12"/>
       <c r="B27" s="4" t="s">
         <v>290</v>
@@ -18304,17 +18878,20 @@
       <c r="D27" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="19" t="s">
+        <v>495</v>
+      </c>
+      <c r="F27" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="G27" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="H27" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="225" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" ht="225" x14ac:dyDescent="0.45">
       <c r="A28" s="12"/>
       <c r="B28" s="4" t="s">
         <v>293</v>
@@ -18325,17 +18902,20 @@
       <c r="D28" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="19" t="s">
+        <v>496</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="G28" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="H28" s="4" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="105" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" ht="105" x14ac:dyDescent="0.45">
       <c r="A29" s="12"/>
       <c r="B29" s="4" t="s">
         <v>298</v>
@@ -18346,17 +18926,20 @@
       <c r="D29" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="19" t="s">
+        <v>497</v>
+      </c>
+      <c r="F29" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="G29" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="H29" s="4" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="270" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" ht="270" x14ac:dyDescent="0.45">
       <c r="A30" s="12"/>
       <c r="B30" s="4" t="s">
         <v>302</v>
@@ -18367,17 +18950,20 @@
       <c r="D30" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="19" t="s">
+        <v>498</v>
+      </c>
+      <c r="F30" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="G30" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="H30" s="4" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="180" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" ht="180" x14ac:dyDescent="0.45">
       <c r="A31" s="12"/>
       <c r="B31" s="4" t="s">
         <v>305</v>
@@ -18388,17 +18974,20 @@
       <c r="D31" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="19" t="s">
+        <v>476</v>
+      </c>
+      <c r="F31" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="G31" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="G31" s="4" t="s">
+      <c r="H31" s="4" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="150" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:8" ht="150" x14ac:dyDescent="0.45">
       <c r="A32" s="12"/>
       <c r="B32" s="4" t="s">
         <v>308</v>
@@ -18409,17 +18998,20 @@
       <c r="D32" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="19" t="s">
+        <v>499</v>
+      </c>
+      <c r="F32" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="G32" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="H32" s="4" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="165" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" ht="165" x14ac:dyDescent="0.45">
       <c r="A33" s="12"/>
       <c r="B33" s="4" t="s">
         <v>313</v>
@@ -18430,17 +19022,20 @@
       <c r="D33" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="19" t="s">
+        <v>500</v>
+      </c>
+      <c r="F33" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="G33" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="H33" s="4" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="120" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:8" ht="120" x14ac:dyDescent="0.45">
       <c r="A34" s="12"/>
       <c r="B34" s="4" t="s">
         <v>316</v>
@@ -18451,17 +19046,20 @@
       <c r="D34" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="19" t="s">
+        <v>477</v>
+      </c>
+      <c r="F34" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="F34" s="4" t="s">
+      <c r="G34" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="G34" s="4" t="s">
+      <c r="H34" s="4" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="165" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:8" ht="165" x14ac:dyDescent="0.45">
       <c r="A35" s="12"/>
       <c r="B35" s="4" t="s">
         <v>320</v>
@@ -18472,17 +19070,20 @@
       <c r="D35" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="19" t="s">
+        <v>501</v>
+      </c>
+      <c r="F35" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="G35" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="G35" s="4" t="s">
+      <c r="H35" s="4" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="120" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:8" ht="120" x14ac:dyDescent="0.45">
       <c r="A36" s="12"/>
       <c r="B36" s="4" t="s">
         <v>127</v>
@@ -18493,17 +19094,20 @@
       <c r="D36" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="19" t="s">
+        <v>502</v>
+      </c>
+      <c r="F36" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="G36" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G36" s="4" t="s">
+      <c r="H36" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="90" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:8" ht="90" x14ac:dyDescent="0.45">
       <c r="A37" s="12"/>
       <c r="B37" s="4" t="s">
         <v>323</v>
@@ -18514,17 +19118,20 @@
       <c r="D37" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="19" t="s">
+        <v>503</v>
+      </c>
+      <c r="F37" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="G37" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="H37" s="4" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="150" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:8" ht="150" x14ac:dyDescent="0.45">
       <c r="A38" s="12"/>
       <c r="B38" s="4" t="s">
         <v>327</v>
@@ -18535,17 +19142,20 @@
       <c r="D38" s="15" t="s">
         <v>201</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E38" s="19" t="s">
+        <v>504</v>
+      </c>
+      <c r="F38" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="G38" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="G38" s="4" t="s">
+      <c r="H38" s="4" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="147.6" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:8" ht="147.6" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="12"/>
       <c r="B39" s="4" t="s">
         <v>331</v>
@@ -18556,17 +19166,20 @@
       <c r="D39" s="15" t="s">
         <v>202</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E39" s="19" t="s">
+        <v>505</v>
+      </c>
+      <c r="F39" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="G39" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="G39" s="4" t="s">
+      <c r="H39" s="4" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="195" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:8" ht="195" x14ac:dyDescent="0.45">
       <c r="A40" s="12"/>
       <c r="B40" s="4" t="s">
         <v>337</v>
@@ -18577,17 +19190,20 @@
       <c r="D40" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E40" s="19" t="s">
+        <v>506</v>
+      </c>
+      <c r="F40" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="G40" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="G40" s="4" t="s">
+      <c r="H40" s="4" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="165" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:8" ht="165" x14ac:dyDescent="0.45">
       <c r="A41" s="12"/>
       <c r="B41" s="4" t="s">
         <v>341</v>
@@ -18598,17 +19214,20 @@
       <c r="D41" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E41" s="19" t="s">
+        <v>507</v>
+      </c>
+      <c r="F41" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="G41" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="G41" s="4" t="s">
+      <c r="H41" s="4" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="120" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:8" ht="120" x14ac:dyDescent="0.45">
       <c r="A42" s="12"/>
       <c r="B42" s="4" t="s">
         <v>118</v>
@@ -18619,17 +19238,20 @@
       <c r="D42" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" s="19" t="s">
+        <v>470</v>
+      </c>
+      <c r="F42" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="G42" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="G42" s="4" t="s">
+      <c r="H42" s="4" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="120" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:8" ht="120" x14ac:dyDescent="0.45">
       <c r="A43" s="12"/>
       <c r="B43" s="4" t="s">
         <v>332</v>
@@ -18640,17 +19262,20 @@
       <c r="D43" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="E43" s="19" t="s">
+        <v>508</v>
+      </c>
+      <c r="F43" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="G43" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="G43" s="4" t="s">
+      <c r="H43" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="105" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:8" ht="105" x14ac:dyDescent="0.45">
       <c r="A44" s="12"/>
       <c r="B44" s="4" t="s">
         <v>333</v>
@@ -18661,17 +19286,20 @@
       <c r="D44" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E44" s="19" t="s">
+        <v>509</v>
+      </c>
+      <c r="F44" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="G44" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="G44" s="4" t="s">
+      <c r="H44" s="4" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="105" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:8" ht="105" x14ac:dyDescent="0.45">
       <c r="A45" s="12"/>
       <c r="B45" s="4" t="s">
         <v>344</v>
@@ -18682,17 +19310,20 @@
       <c r="D45" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="E45" s="19" t="s">
+        <v>510</v>
+      </c>
+      <c r="F45" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="F45" s="4" t="s">
+      <c r="G45" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="G45" s="4" t="s">
+      <c r="H45" s="4" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="120" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:8" ht="120" x14ac:dyDescent="0.45">
       <c r="A46" s="12"/>
       <c r="B46" s="4" t="s">
         <v>345</v>
@@ -18703,17 +19334,20 @@
       <c r="D46" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E46" s="19" t="s">
+        <v>475</v>
+      </c>
+      <c r="F46" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="F46" s="4" t="s">
+      <c r="G46" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="G46" s="4" t="s">
+      <c r="H46" s="4" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="89.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:8" ht="89.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="12"/>
       <c r="B47" s="4" t="s">
         <v>346</v>
@@ -18724,17 +19358,20 @@
       <c r="D47" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="E47" s="19" t="s">
+        <v>511</v>
+      </c>
+      <c r="F47" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="F47" s="4" t="s">
+      <c r="G47" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="G47" s="4" t="s">
+      <c r="H47" s="4" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="120" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:8" ht="120" x14ac:dyDescent="0.45">
       <c r="A48" s="12"/>
       <c r="B48" s="4" t="s">
         <v>347</v>
@@ -18745,17 +19382,20 @@
       <c r="D48" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="E48" s="19" t="s">
+        <v>512</v>
+      </c>
+      <c r="F48" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="F48" s="4" t="s">
+      <c r="G48" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="G48" s="4" t="s">
+      <c r="H48" s="4" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="120" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:8" ht="120" x14ac:dyDescent="0.45">
       <c r="A49" s="12"/>
       <c r="B49" s="4" t="s">
         <v>348</v>
@@ -18766,17 +19406,20 @@
       <c r="D49" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="E49" s="4" t="s">
+      <c r="E49" s="19" t="s">
+        <v>513</v>
+      </c>
+      <c r="F49" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="F49" s="4" t="s">
+      <c r="G49" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="G49" s="4" t="s">
+      <c r="H49" s="4" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="120" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:8" ht="120" x14ac:dyDescent="0.45">
       <c r="A50" s="13"/>
       <c r="B50" s="4" t="s">
         <v>349</v>
@@ -18787,13 +19430,16 @@
       <c r="D50" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="E50" s="19" t="s">
+        <v>514</v>
+      </c>
+      <c r="F50" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="F50" s="4" t="s">
+      <c r="G50" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="G50" s="4" t="s">
+      <c r="H50" s="4" t="s">
         <v>369</v>
       </c>
     </row>
@@ -18855,10 +19501,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0052A72F-99A5-4DB1-A333-01DE0A789EB0}">
-  <dimension ref="A3:G14"/>
+  <dimension ref="A3:H14"/>
   <sheetViews>
     <sheetView topLeftCell="B12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E12" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -18867,18 +19513,19 @@
     <col min="2" max="2" width="19.5" style="3" customWidth="1"/>
     <col min="3" max="3" width="15.5" style="3" customWidth="1"/>
     <col min="4" max="4" width="28.8984375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="39.59765625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="29.3984375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="42.19921875" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="8.796875" style="3"/>
+    <col min="5" max="5" width="39.59765625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="39.59765625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="29.3984375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="42.19921875" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="8.796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D3" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>171</v>
       </c>
@@ -18891,17 +19538,20 @@
       <c r="D5" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="18" t="s">
+        <v>440</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="120" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" ht="120" x14ac:dyDescent="0.45">
       <c r="A6" s="11" t="s">
         <v>54</v>
       </c>
@@ -18914,17 +19564,20 @@
       <c r="D6" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="19" t="s">
+        <v>515</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="150" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" ht="150" x14ac:dyDescent="0.45">
       <c r="A7" s="12"/>
       <c r="B7" s="9" t="s">
         <v>106</v>
@@ -18935,17 +19588,20 @@
       <c r="D7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="19" t="s">
+        <v>457</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="165" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" ht="165" x14ac:dyDescent="0.45">
       <c r="A8" s="12"/>
       <c r="B8" s="9" t="s">
         <v>107</v>
@@ -18956,17 +19612,20 @@
       <c r="D8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="19" t="s">
+        <v>458</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="135" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" ht="135" x14ac:dyDescent="0.45">
       <c r="A9" s="12"/>
       <c r="B9" s="9" t="s">
         <v>108</v>
@@ -18977,17 +19636,20 @@
       <c r="D9" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="19" t="s">
+        <v>459</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="150" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" ht="150" x14ac:dyDescent="0.45">
       <c r="A10" s="12"/>
       <c r="B10" s="9" t="s">
         <v>109</v>
@@ -18998,17 +19660,20 @@
       <c r="D10" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="19" t="s">
+        <v>460</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="150" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" ht="150" x14ac:dyDescent="0.45">
       <c r="A11" s="12"/>
       <c r="B11" s="9" t="s">
         <v>126</v>
@@ -19019,17 +19684,20 @@
       <c r="D11" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="19" t="s">
+        <v>516</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="210" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" ht="210" x14ac:dyDescent="0.45">
       <c r="A12" s="12"/>
       <c r="B12" s="9" t="s">
         <v>260</v>
@@ -19040,17 +19708,20 @@
       <c r="D12" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="19" t="s">
+        <v>488</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="H12" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="159.6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" ht="225" x14ac:dyDescent="0.45">
       <c r="A13" s="12"/>
       <c r="B13" s="9" t="s">
         <v>114</v>
@@ -19061,17 +19732,20 @@
       <c r="D13" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="19" t="s">
+        <v>517</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="G13" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="120" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" ht="120" x14ac:dyDescent="0.45">
       <c r="A14" s="13"/>
       <c r="B14" s="9" t="s">
         <v>127</v>
@@ -19082,13 +19756,16 @@
       <c r="D14" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="19" t="s">
+        <v>502</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>439</v>
       </c>
     </row>
@@ -19114,10 +19791,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6EC331A-EAD8-4B76-BCAE-035C1A04ED8C}">
-  <dimension ref="A3:G20"/>
+  <dimension ref="A3:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -19126,18 +19803,19 @@
     <col min="2" max="2" width="19.5" style="3" customWidth="1"/>
     <col min="3" max="3" width="15.5" style="3" customWidth="1"/>
     <col min="4" max="4" width="28.8984375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="39.59765625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="29.3984375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="42.19921875" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="8.796875" style="3"/>
+    <col min="5" max="5" width="39.59765625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="39.59765625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="29.3984375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="42.19921875" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="8.796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D3" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>171</v>
       </c>
@@ -19150,17 +19828,20 @@
       <c r="D5" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="18" t="s">
+        <v>440</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="135" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" ht="135" x14ac:dyDescent="0.45">
       <c r="A6" s="11" t="s">
         <v>370</v>
       </c>
@@ -19171,17 +19852,20 @@
       <c r="D6" s="16" t="s">
         <v>371</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="19" t="s">
+        <v>441</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="144.6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" ht="165" x14ac:dyDescent="0.45">
       <c r="A7" s="12"/>
       <c r="B7" s="4" t="s">
         <v>383</v>
@@ -19192,17 +19876,20 @@
       <c r="D7" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="19" t="s">
+        <v>442</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="105" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" ht="105" x14ac:dyDescent="0.45">
       <c r="A8" s="12"/>
       <c r="B8" s="4" t="s">
         <v>384</v>
@@ -19211,17 +19898,20 @@
       <c r="D8" s="16" t="s">
         <v>372</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="19" t="s">
+        <v>443</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="120" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" ht="120" x14ac:dyDescent="0.45">
       <c r="A9" s="12"/>
       <c r="B9" s="4" t="s">
         <v>385</v>
@@ -19230,17 +19920,20 @@
       <c r="D9" s="16" t="s">
         <v>373</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="19" t="s">
+        <v>444</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>403</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="135" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" ht="135" x14ac:dyDescent="0.45">
       <c r="A10" s="12"/>
       <c r="B10" s="4" t="s">
         <v>386</v>
@@ -19249,17 +19942,20 @@
       <c r="D10" s="16" t="s">
         <v>374</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="19" t="s">
+        <v>445</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="165" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" ht="165" x14ac:dyDescent="0.45">
       <c r="A11" s="12"/>
       <c r="B11" s="4" t="s">
         <v>387</v>
@@ -19268,17 +19964,20 @@
       <c r="D11" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="19" t="s">
+        <v>446</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="180" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" ht="180" x14ac:dyDescent="0.45">
       <c r="A12" s="12"/>
       <c r="B12" s="4" t="s">
         <v>388</v>
@@ -19287,17 +19986,20 @@
       <c r="D12" s="16" t="s">
         <v>375</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="19" t="s">
+        <v>447</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="H12" s="4" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="165" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" ht="165" x14ac:dyDescent="0.45">
       <c r="A13" s="12"/>
       <c r="B13" s="4" t="s">
         <v>389</v>
@@ -19306,17 +20008,20 @@
       <c r="D13" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="19" t="s">
+        <v>448</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>413</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="G13" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="285" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" ht="285" x14ac:dyDescent="0.45">
       <c r="A14" s="12"/>
       <c r="B14" s="4" t="s">
         <v>392</v>
@@ -19327,17 +20032,20 @@
       <c r="D14" s="16" t="s">
         <v>377</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="19" t="s">
+        <v>449</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>416</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="270" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" ht="270" x14ac:dyDescent="0.45">
       <c r="A15" s="12"/>
       <c r="B15" s="4" t="s">
         <v>390</v>
@@ -19348,17 +20056,20 @@
       <c r="D15" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="G15" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="H15" s="4" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="255" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" ht="255" x14ac:dyDescent="0.45">
       <c r="A16" s="12"/>
       <c r="B16" s="4" t="s">
         <v>395</v>
@@ -19369,17 +20080,20 @@
       <c r="D16" s="16" t="s">
         <v>378</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>420</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>421</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="H16" s="4" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="225" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" ht="225" x14ac:dyDescent="0.45">
       <c r="A17" s="12"/>
       <c r="B17" s="4" t="s">
         <v>393</v>
@@ -19388,17 +20102,20 @@
       <c r="D17" s="16" t="s">
         <v>379</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="19" t="s">
+        <v>452</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>423</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="G17" s="4" t="s">
         <v>424</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="H17" s="4" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="240" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" ht="240" x14ac:dyDescent="0.45">
       <c r="A18" s="12"/>
       <c r="B18" s="4" t="s">
         <v>391</v>
@@ -19407,17 +20124,20 @@
       <c r="D18" s="16" t="s">
         <v>380</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="19" t="s">
+        <v>453</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="G18" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="H18" s="4" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="120" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" ht="120" x14ac:dyDescent="0.45">
       <c r="A19" s="12"/>
       <c r="B19" s="4" t="s">
         <v>119</v>
@@ -19428,17 +20148,20 @@
       <c r="D19" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="19" t="s">
+        <v>454</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="G19" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="H19" s="4" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="225" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" ht="225" x14ac:dyDescent="0.45">
       <c r="A20" s="13"/>
       <c r="B20" s="4" t="s">
         <v>394</v>
@@ -19449,13 +20172,16 @@
       <c r="D20" s="16" t="s">
         <v>381</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="19" t="s">
+        <v>455</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>429</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="G20" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="H20" s="4" t="s">
         <v>431</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added SBOM paper information
</commit_message>
<xml_diff>
--- a/subgroups/sbom-sg/outcomes/SBOM/SBOMTools/LearnSBOM/LearnSBOMList.xlsx
+++ b/subgroups/sbom-sg/outcomes/SBOM/SBOMTools/LearnSBOM/LearnSBOMList.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sonyjpn-my.sharepoint.com/personal/hiroyuki_fukuchi_sony_com/Documents/ドキュメント/OpenChain/SBOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="609" documentId="8_{0F481742-EC34-4620-BA6D-267154DAC474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9479E97-C23A-470B-9ABE-3B3E8793D418}"/>
+  <xr:revisionPtr revIDLastSave="716" documentId="8_{0F481742-EC34-4620-BA6D-267154DAC474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CF191AB-EF0A-433A-A0FC-C9561A164D6E}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="1464" windowWidth="20772" windowHeight="10152" activeTab="3" xr2:uid="{627C03B7-2A37-4A7C-9FB2-07470DF8D28A}"/>
+    <workbookView xWindow="2952" yWindow="720" windowWidth="20772" windowHeight="11280" firstSheet="1" activeTab="4" xr2:uid="{627C03B7-2A37-4A7C-9FB2-07470DF8D28A}"/>
   </bookViews>
   <sheets>
     <sheet name="SBOM_Utility_Tools" sheetId="2" r:id="rId1"/>
     <sheet name="SBOM_Generator" sheetId="4" r:id="rId2"/>
     <sheet name="SBOM_Converters" sheetId="3" r:id="rId3"/>
     <sheet name="Security_Tools" sheetId="5" r:id="rId4"/>
-    <sheet name="SBOM_Info" sheetId="1" r:id="rId5"/>
+    <sheet name="SBOM関連情報" sheetId="6" r:id="rId5"/>
+    <sheet name="SBOM_Info" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="548">
   <si>
     <t>https://www.youtube.com/@LearnSBOM/playlistsその他は以下です。</t>
   </si>
@@ -8508,12 +8509,150 @@
     </r>
     <phoneticPr fontId="10"/>
   </si>
+  <si>
+    <t>https://www.finna.fi/Record/trepo.10024_148790</t>
+  </si>
+  <si>
+    <t>Managing 3rd Party Software Components with Software Bill of Materials</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ドイツの情報セキュリティ庁によるSBOMの要件定義</t>
+  </si>
+  <si>
+    <t>SBOM-Anforderungen: TR-03183-2 stärkt Sicherheit in der Software-Lieferkette</t>
+  </si>
+  <si>
+    <t>https://spdx.dev/a-step-by-step-guide-to-signing-an-spdx-sbom-with-sigstores-cosign/</t>
+  </si>
+  <si>
+    <t>https://www.contrastsecurity.com/security-influencers/sbom-quality-cyclonedx-and-the-5-dimensions-of-sbom-quality-contrast-security</t>
+  </si>
+  <si>
+    <t>SBOM Quality: CycloneDX and the 5 dimensions of SBOM quality | Contrast Security</t>
+  </si>
+  <si>
+    <t>https://cyclonedx.org/docs/1.5/json/ </t>
+  </si>
+  <si>
+    <t>https://www.publickey1.jp/blog/23/githubcomsbomsbom.html</t>
+  </si>
+  <si>
+    <t>Top 7 SBOM Generation Tools and How to Choose</t>
+  </si>
+  <si>
+    <t>解説</t>
+    <rPh sb="0" eb="2">
+      <t>カイセツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>日本語概要</t>
+    <rPh sb="0" eb="5">
+      <t>ニホンゴガイヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>英文概要</t>
+    <rPh sb="0" eb="4">
+      <t>エイブンガイヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SBOM定義</t>
+    <rPh sb="4" eb="6">
+      <t>テイギ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CycloneDX v1.5</t>
+  </si>
+  <si>
+    <t>CycloneDX v1.5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>URL</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>カテゴリ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2303.11102</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2301.05362</t>
+  </si>
+  <si>
+    <t>論文</t>
+    <rPh sb="0" eb="2">
+      <t>ロンブン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>論文</t>
+    <rPh sb="0" eb="2">
+      <t>ロンブン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Debianパッケージに対する依存関係を含むSPDXファイルの自動生成ツール</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SBOMによる3rdPartyソフトウェアパッケージ管理</t>
+    <rPh sb="26" eb="28">
+      <t>カンリ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Challenges of Producing Software Bill Of Materials for Java</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>An Empirical Study on Software Bill of Materials: Where We Stand and the Road Ahead</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://ken.ieice.org/ken/paper/20220730sCLt/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>a tool to automatically generate SPDX files including dependency descriptions for Debian packages</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>JavaのSBOM生成について</t>
+    <rPh sb="9" eb="11">
+      <t>セイセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SBOMに関する実証研究</t>
+    <rPh sb="5" eb="6">
+      <t>カン</t>
+    </rPh>
+    <rPh sb="8" eb="12">
+      <t>ジッショウケンキュウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8591,6 +8730,14 @@
       <name val="游ゴシック"/>
       <family val="3"/>
       <charset val="128"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -8698,7 +8845,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -8757,6 +8904,18 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -19503,7 +19662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0052A72F-99A5-4DB1-A333-01DE0A789EB0}">
   <dimension ref="A3:H14"/>
   <sheetViews>
-    <sheetView topLeftCell="B12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="B10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E12" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
@@ -19793,7 +19952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6EC331A-EAD8-4B76-BCAE-035C1A04ED8C}">
   <dimension ref="A3:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -20212,11 +20371,266 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C88F823-0D1C-4815-80D1-40AD63B22AC6}">
+  <dimension ref="A2:D23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="2" width="31" style="20" customWidth="1"/>
+    <col min="3" max="3" width="37.3984375" style="20" customWidth="1"/>
+    <col min="4" max="4" width="42.19921875" style="20" customWidth="1"/>
+    <col min="5" max="5" width="43" style="20" customWidth="1"/>
+    <col min="6" max="16384" width="8.796875" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="21" t="s">
+        <v>535</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>529</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>530</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.45">
+      <c r="A3" s="22" t="s">
+        <v>538</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>541</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>519</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.45">
+      <c r="A4" s="22" t="s">
+        <v>539</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>540</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>545</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.45">
+      <c r="A5" s="22" t="s">
+        <v>539</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>546</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>542</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.45">
+      <c r="A6" s="22" t="s">
+        <v>539</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>547</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>543</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+    </row>
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.45">
+      <c r="A10" s="22" t="s">
+        <v>531</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>520</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>521</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" s="23"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+    </row>
+    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.45">
+      <c r="A14" s="22" t="s">
+        <v>528</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.45">
+      <c r="A15" s="22" t="s">
+        <v>528</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.45">
+      <c r="A16" s="22" t="s">
+        <v>528</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>524</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17" s="22" t="s">
+        <v>528</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>533</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.45">
+      <c r="A18" s="22" t="s">
+        <v>528</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>532</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" s="22" t="s">
+        <v>528</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>532</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.45">
+      <c r="A20" s="22" t="s">
+        <v>528</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.45">
+      <c r="A21" s="22" t="s">
+        <v>528</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>527</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>527</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{9780DF05-8584-4CCB-B703-1E03AF32991F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB8526CA-8E14-4BA8-BAA5-3C86D2FD4276}">
   <dimension ref="B2:D34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
updated SBOM paper information
</commit_message>
<xml_diff>
--- a/subgroups/sbom-sg/outcomes/SBOM/SBOMTools/LearnSBOM/LearnSBOMList.xlsx
+++ b/subgroups/sbom-sg/outcomes/SBOM/SBOMTools/LearnSBOM/LearnSBOMList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sonyjpn-my.sharepoint.com/personal/hiroyuki_fukuchi_sony_com/Documents/ドキュメント/OpenChain/SBOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="716" documentId="8_{0F481742-EC34-4620-BA6D-267154DAC474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CF191AB-EF0A-433A-A0FC-C9561A164D6E}"/>
+  <xr:revisionPtr revIDLastSave="722" documentId="8_{0F481742-EC34-4620-BA6D-267154DAC474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D64FF335-595A-4ECD-8473-81033B00F418}"/>
   <bookViews>
-    <workbookView xWindow="2952" yWindow="720" windowWidth="20772" windowHeight="11280" firstSheet="1" activeTab="4" xr2:uid="{627C03B7-2A37-4A7C-9FB2-07470DF8D28A}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="20772" windowHeight="11280" firstSheet="1" activeTab="4" xr2:uid="{627C03B7-2A37-4A7C-9FB2-07470DF8D28A}"/>
   </bookViews>
   <sheets>
     <sheet name="SBOM_Utility_Tools" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="550">
   <si>
     <t>https://www.youtube.com/@LearnSBOM/playlistsその他は以下です。</t>
   </si>
@@ -8645,6 +8645,13 @@
     <rPh sb="8" eb="12">
       <t>ジッショウケンキュウ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Software Bill of Materials Adoption: A Mining Study from GitHub</t>
+  </si>
+  <si>
+    <t>BOMs Away! Inside the Minds of Stakeholders: A Comprehensive Study of Bills of Materials for Software Systems</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -20372,10 +20379,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C88F823-0D1C-4815-80D1-40AD63B22AC6}">
-  <dimension ref="A2:D23"/>
+  <dimension ref="A2:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -20457,99 +20464,99 @@
         <v>537</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7" s="23"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.45">
+      <c r="A7" s="22" t="s">
+        <v>538</v>
+      </c>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22" t="s">
+        <v>548</v>
+      </c>
+      <c r="D7" s="22"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" s="23"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.45">
+      <c r="A8" s="22" t="s">
+        <v>538</v>
+      </c>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22" t="s">
+        <v>549</v>
+      </c>
+      <c r="D8" s="22"/>
     </row>
-    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.45">
-      <c r="A10" s="22" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+    </row>
+    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.45">
+      <c r="A11" s="22" t="s">
         <v>531</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B11" s="22" t="s">
         <v>520</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C11" s="22" t="s">
         <v>521</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D11" s="22" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A12" s="23"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
     </row>
-    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.45">
-      <c r="A14" s="22" t="s">
-        <v>528</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>11</v>
-      </c>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
     </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.45">
       <c r="A15" s="22" t="s">
         <v>528</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="22"/>
+        <v>10</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>18</v>
+      </c>
       <c r="D15" s="22" t="s">
-        <v>522</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.45">
       <c r="A16" s="22" t="s">
         <v>528</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>524</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C16" s="22"/>
       <c r="D16" s="22" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.45">
       <c r="A17" s="22" t="s">
         <v>528</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>533</v>
+        <v>524</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>14</v>
+        <v>523</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="22" t="s">
         <v>528</v>
       </c>
@@ -20557,13 +20564,13 @@
         <v>28</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.45">
       <c r="A19" s="22" t="s">
         <v>528</v>
       </c>
@@ -20574,19 +20581,21 @@
         <v>532</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>525</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="22" t="s">
         <v>528</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="22"/>
+        <v>28</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>532</v>
+      </c>
       <c r="D20" s="22" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.45">
@@ -20594,26 +20603,38 @@
         <v>528</v>
       </c>
       <c r="B21" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.45">
+      <c r="A22" s="22" t="s">
+        <v>528</v>
+      </c>
+      <c r="B22" s="22" t="s">
         <v>527</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C22" s="22" t="s">
         <v>527</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D22" s="22" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="22"/>
       <c r="B23" s="22"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" s="22"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>